<commit_message>
Actualizacion excel de normalizacion
</commit_message>
<xml_diff>
--- a/Normalizaciòn y diseño base de datos proyecto 2.xlsx
+++ b/Normalizaciòn y diseño base de datos proyecto 2.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="47">
   <si>
     <t>Entidades</t>
   </si>
@@ -19,15 +19,27 @@
     <t>usuario</t>
   </si>
   <si>
+    <t>recomendaciones</t>
+  </si>
+  <si>
     <t>multimedia</t>
   </si>
   <si>
+    <t>Genero_Contenido</t>
+  </si>
+  <si>
     <t>subscripcion</t>
   </si>
   <si>
+    <t>anuncios</t>
+  </si>
+  <si>
     <t>perfil</t>
   </si>
   <si>
+    <t>favoritos</t>
+  </si>
+  <si>
     <t>Actor</t>
   </si>
   <si>
@@ -61,28 +73,85 @@
     <t>id</t>
   </si>
   <si>
+    <t>estado_vista</t>
+  </si>
+  <si>
+    <t>estado_perfil</t>
+  </si>
+  <si>
+    <t>premio</t>
+  </si>
+  <si>
+    <t>categoria</t>
+  </si>
+  <si>
+    <t>id_premio</t>
+  </si>
+  <si>
+    <t>nombre_completo</t>
+  </si>
+  <si>
+    <t>Multimedia</t>
+  </si>
+  <si>
+    <t>Subscripcion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          </t>
+  </si>
+  <si>
+    <t>Fecha_Estreno</t>
+  </si>
+  <si>
+    <t>Tipo_Contenido</t>
+  </si>
+  <si>
+    <t>links</t>
+  </si>
+  <si>
+    <t>tipo</t>
+  </si>
+  <si>
+    <t>fecha_vencimiento</t>
+  </si>
+  <si>
+    <t>Recomendaciones</t>
+  </si>
+  <si>
+    <t>perfil_id</t>
+  </si>
+  <si>
+    <t>contenido_id</t>
+  </si>
+  <si>
+    <t>id_genero</t>
+  </si>
+  <si>
+    <t>nombre</t>
+  </si>
+  <si>
+    <t>id_contenido</t>
+  </si>
+  <si>
+    <t>id_usuario</t>
+  </si>
+  <si>
+    <t>id_anuncio</t>
+  </si>
+  <si>
+    <t>nombre_anunciante</t>
+  </si>
+  <si>
+    <t>actor_contenido</t>
+  </si>
+  <si>
+    <t>director_contenido</t>
+  </si>
+  <si>
+    <t>premios_contenido</t>
+  </si>
+  <si>
     <t>multimedia_id</t>
-  </si>
-  <si>
-    <t>premio</t>
-  </si>
-  <si>
-    <t>categoria</t>
-  </si>
-  <si>
-    <t>Multimedia</t>
-  </si>
-  <si>
-    <t>Fecha_Estreno</t>
-  </si>
-  <si>
-    <t>Tipo_Contenido</t>
-  </si>
-  <si>
-    <t>links</t>
-  </si>
-  <si>
-    <t>nombre_completo</t>
   </si>
 </sst>
 </file>
@@ -137,7 +206,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -150,13 +219,10 @@
     <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -374,6 +440,9 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="2" max="2" width="16.29"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
@@ -384,130 +453,283 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
+      <c r="B2" s="2" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>3</v>
+        <v>5</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="s">
-        <v>8</v>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="2" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="3" t="s">
-        <v>9</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="E12" s="4"/>
       <c r="G12" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="M12" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q12" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="K12" s="4" t="s">
-        <v>7</v>
-      </c>
+      <c r="S12" s="4"/>
     </row>
     <row r="13">
       <c r="A13" s="5" t="s">
         <v>1</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="E13" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G13" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="G13" s="5" t="s">
-        <v>9</v>
-      </c>
       <c r="H13" s="5" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="I13" s="5" t="s">
-        <v>15</v>
+        <v>19</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>20</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="L13" s="2" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="M13" s="2" t="s">
-        <v>18</v>
+        <v>22</v>
+      </c>
+      <c r="N13" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="O13" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q13" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="R13" s="2" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F16" s="6"/>
-      <c r="G16" s="4" t="s">
-        <v>5</v>
+        <v>26</v>
+      </c>
+      <c r="F16" s="4"/>
+      <c r="G16" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I16" s="4"/>
+      <c r="K16" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="P16" s="2" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="5" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="I17" s="2" t="s">
-        <v>23</v>
+        <v>25</v>
+      </c>
+      <c r="K17" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="L17" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="M17" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="N17" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="K19" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q19" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="K20" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="L20" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="M20" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="N20" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="O20" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q20" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="R20" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="S20" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="T20" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="A12:E12"/>
-    <mergeCell ref="G12:I12"/>
-    <mergeCell ref="K12:M12"/>
+  <mergeCells count="16">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A12:D12"/>
+    <mergeCell ref="G12:K12"/>
+    <mergeCell ref="K16:N16"/>
+    <mergeCell ref="Q12:R12"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="M12:O12"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="G22:H22"/>
     <mergeCell ref="A16:E16"/>
-    <mergeCell ref="G16:I16"/>
+    <mergeCell ref="A19:C19"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="K19:O19"/>
+    <mergeCell ref="Q19:T19"/>
+    <mergeCell ref="A22:B22"/>
   </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>